<commit_message>
pitaya funcioanndo el scroll
</commit_message>
<xml_diff>
--- a/documentacion/Actividades Desarrollo Proyecto.xlsx
+++ b/documentacion/Actividades Desarrollo Proyecto.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Analisis y concepción" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Actividad</t>
   </si>
@@ -55,6 +55,21 @@
   </si>
   <si>
     <t>Desarrollar páginas estaticas y plantilla de la aplicación</t>
+  </si>
+  <si>
+    <t>front-end slider</t>
+  </si>
+  <si>
+    <t>front galeria de fondos miembros</t>
+  </si>
+  <si>
+    <t>front galeria de fondos publico</t>
+  </si>
+  <si>
+    <t>front end vista de galeria con overlay</t>
+  </si>
+  <si>
+    <t>back end crud de menus hubo cambios</t>
   </si>
 </sst>
 </file>
@@ -398,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,25 +434,40 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -447,10 +477,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,12 +506,18 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>11</v>
       </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -492,10 +528,41 @@
       <c r="B5" t="s">
         <v>12</v>
       </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>